<commit_message>
IBM updated stats for US and UK english
</commit_message>
<xml_diff>
--- a/IBM_summary.xlsx
+++ b/IBM_summary.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah/Downloads/105-project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah/Downloads/CS105-Speech-Algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C00D99C-B5A1-FF43-BA66-34CC2FDFF834}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B81C10-698F-5C47-8F01-807719865964}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="2080" windowWidth="17540" windowHeight="13900" xr2:uid="{650F48BB-91CC-1B44-8AC3-03014BB38A08}"/>
+    <workbookView xWindow="11260" yWindow="2120" windowWidth="17540" windowHeight="13900" xr2:uid="{650F48BB-91CC-1B44-8AC3-03014BB38A08}"/>
   </bookViews>
   <sheets>
     <sheet name="IBM data" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>German</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Category</t>
+  </si>
+  <si>
+    <t>US English</t>
+  </si>
+  <si>
+    <t>UK English</t>
   </si>
 </sst>
 </file>
@@ -459,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13C59EBF-BEA4-1940-B406-2CE00ACBA3ED}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -816,6 +822,52 @@
         <v>89.4</v>
       </c>
     </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="D17" s="1">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="F17">
+        <v>6.6</v>
+      </c>
+      <c r="G17">
+        <v>6.5</v>
+      </c>
+      <c r="I17">
+        <v>9.6</v>
+      </c>
+      <c r="J17">
+        <v>90.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="1">
+        <v>26.9</v>
+      </c>
+      <c r="D18" s="1">
+        <v>11.9</v>
+      </c>
+      <c r="F18">
+        <v>8.6</v>
+      </c>
+      <c r="G18">
+        <v>4.2</v>
+      </c>
+      <c r="I18">
+        <v>12.5</v>
+      </c>
+      <c r="J18">
+        <v>87.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>